<commit_message>
fixed issues with reading excel files, removed csv
</commit_message>
<xml_diff>
--- a/questions.xlsx
+++ b/questions.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23029"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sadar\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\work\BE PROJECT\Computerised-adaptive-assesments\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{7F03B368-2149-4020-8BDA-66F6AC6312F3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F9282ABA-7B84-4148-A3F5-858E915B634C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="questions" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="60">
   <si>
     <t>The wages of 10 workers for a six-day week is $ 1200. What are the one day’s wages of 4 workers?</t>
   </si>
@@ -38,9 +38,6 @@
   </si>
   <si>
     <t>integer</t>
-  </si>
-  <si>
-    <t>whole</t>
   </si>
   <si>
     <t xml:space="preserve">A clock strikes once at 1 o’clock, twice at 2 o’clock, thrice at 3 o’clock and so on. How many times will it strike in 24 hours? </t>
@@ -198,11 +195,20 @@
   <si>
     <t xml:space="preserve">Complete the following sequence. 2, 3, 5, 9, _____, 33 </t>
   </si>
+  <si>
+    <t>A</t>
+  </si>
+  <si>
+    <t>C</t>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1042,10 +1048,12 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F2" sqref="F2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1065,8 +1073,8 @@
       <c r="D1">
         <v>80</v>
       </c>
-      <c r="F1">
-        <v>80</v>
+      <c r="F1" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
@@ -1082,8 +1090,8 @@
       <c r="D2">
         <v>0</v>
       </c>
-      <c r="F2">
-        <v>1</v>
+      <c r="F2" t="s">
+        <v>59</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
@@ -1100,12 +1108,12 @@
         <v>5</v>
       </c>
       <c r="F3" t="s">
-        <v>6</v>
+        <v>57</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B4">
         <v>78</v>
@@ -1116,30 +1124,30 @@
       <c r="D4">
         <v>156</v>
       </c>
-      <c r="F4">
-        <v>156</v>
+      <c r="F4" t="s">
+        <v>58</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
+        <v>7</v>
+      </c>
+      <c r="B5" t="s">
         <v>8</v>
       </c>
-      <c r="B5" t="s">
+      <c r="C5" t="s">
         <v>9</v>
       </c>
-      <c r="C5" t="s">
+      <c r="D5" t="s">
         <v>10</v>
       </c>
-      <c r="D5" t="s">
-        <v>11</v>
-      </c>
       <c r="F5" t="s">
-        <v>10</v>
+        <v>59</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B6">
         <v>15</v>
@@ -1150,13 +1158,13 @@
       <c r="D6">
         <v>12</v>
       </c>
-      <c r="F6">
-        <v>15</v>
+      <c r="F6" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B7">
         <v>1</v>
@@ -1167,13 +1175,13 @@
       <c r="D7">
         <v>8</v>
       </c>
-      <c r="F7">
-        <v>1</v>
+      <c r="F7" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B8" s="1">
         <v>0.64236111111111105</v>
@@ -1184,13 +1192,13 @@
       <c r="D8" s="1">
         <v>0.12847222222222224</v>
       </c>
-      <c r="F8" s="1">
-        <v>0.12847222222222224</v>
+      <c r="F8" s="1" t="s">
+        <v>58</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B9">
         <v>60</v>
@@ -1201,13 +1209,13 @@
       <c r="D9">
         <v>62</v>
       </c>
-      <c r="F9">
-        <v>60</v>
+      <c r="F9" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B10">
         <v>4</v>
@@ -1218,13 +1226,13 @@
       <c r="D10">
         <v>10</v>
       </c>
-      <c r="F10">
-        <v>4</v>
+      <c r="F10" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B11">
         <v>27</v>
@@ -1235,13 +1243,13 @@
       <c r="D11">
         <v>125</v>
       </c>
-      <c r="F11">
-        <v>100</v>
+      <c r="F11" t="s">
+        <v>59</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B12">
         <v>7</v>
@@ -1252,13 +1260,13 @@
       <c r="D12">
         <v>25</v>
       </c>
-      <c r="F12">
-        <v>10</v>
+      <c r="F12" t="s">
+        <v>59</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B13" s="1">
         <v>0.5854166666666667</v>
@@ -1269,13 +1277,13 @@
       <c r="D13" s="1">
         <v>8.4027777777777771E-2</v>
       </c>
-      <c r="F13" s="1">
-        <v>8.4027777777777771E-2</v>
+      <c r="F13" s="1" t="s">
+        <v>58</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B14">
         <v>0.06</v>
@@ -1286,13 +1294,13 @@
       <c r="D14" s="2">
         <v>6.0000000000000002E-5</v>
       </c>
-      <c r="F14" s="2">
-        <v>6.0000000000000002E-5</v>
+      <c r="F14" s="2" t="s">
+        <v>58</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B15">
         <v>26</v>
@@ -1303,13 +1311,13 @@
       <c r="D15">
         <v>28</v>
       </c>
-      <c r="F15">
-        <v>32</v>
+      <c r="F15" t="s">
+        <v>59</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B16">
         <v>7</v>
@@ -1320,13 +1328,13 @@
       <c r="D16">
         <v>9</v>
       </c>
-      <c r="F16">
-        <v>7</v>
+      <c r="F16" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B17">
         <v>6</v>
@@ -1337,13 +1345,13 @@
       <c r="D17">
         <v>3</v>
       </c>
-      <c r="F17">
-        <v>4</v>
+      <c r="F17" t="s">
+        <v>59</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B18" s="3">
         <v>0.8</v>
@@ -1354,13 +1362,13 @@
       <c r="D18" s="3">
         <v>0.14000000000000001</v>
       </c>
-      <c r="F18" s="3">
-        <v>0.2</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F18" s="3" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" ht="60" x14ac:dyDescent="0.25">
       <c r="A19" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B19">
         <v>3</v>
@@ -1371,30 +1379,30 @@
       <c r="D19">
         <v>8</v>
       </c>
-      <c r="F19">
-        <v>3</v>
+      <c r="F19" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
+        <v>25</v>
+      </c>
+      <c r="B20" t="s">
         <v>26</v>
       </c>
-      <c r="B20" t="s">
+      <c r="C20" t="s">
         <v>27</v>
       </c>
-      <c r="C20" t="s">
+      <c r="D20" t="s">
         <v>28</v>
       </c>
-      <c r="D20" t="s">
-        <v>29</v>
-      </c>
       <c r="F20" t="s">
-        <v>29</v>
+        <v>58</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B21">
         <v>5</v>
@@ -1405,13 +1413,13 @@
       <c r="D21">
         <v>10</v>
       </c>
-      <c r="F21">
-        <v>2</v>
+      <c r="F21" t="s">
+        <v>59</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B22">
         <v>4</v>
@@ -1422,13 +1430,13 @@
       <c r="D22">
         <v>16</v>
       </c>
-      <c r="F22">
-        <v>16</v>
+      <c r="F22" t="s">
+        <v>58</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B23">
         <v>1200</v>
@@ -1439,13 +1447,13 @@
       <c r="D23">
         <v>1800</v>
       </c>
-      <c r="F23">
-        <v>1200</v>
+      <c r="F23" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B24">
         <v>1090</v>
@@ -1456,13 +1464,13 @@
       <c r="D24">
         <v>1224</v>
       </c>
-      <c r="F24">
-        <v>1224</v>
+      <c r="F24" t="s">
+        <v>58</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B25">
         <v>11</v>
@@ -1473,13 +1481,13 @@
       <c r="D25">
         <v>15</v>
       </c>
-      <c r="F25">
-        <v>17</v>
+      <c r="F25" t="s">
+        <v>59</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B26">
         <v>40</v>
@@ -1490,13 +1498,13 @@
       <c r="D26">
         <v>60</v>
       </c>
-      <c r="F26">
-        <v>40</v>
+      <c r="F26" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B27">
         <v>852</v>
@@ -1507,13 +1515,13 @@
       <c r="D27">
         <v>568</v>
       </c>
-      <c r="F27">
-        <v>852</v>
+      <c r="F27" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B28">
         <v>15</v>
@@ -1524,13 +1532,13 @@
       <c r="D28">
         <v>75</v>
       </c>
-      <c r="F28">
-        <v>25</v>
+      <c r="F28" t="s">
+        <v>59</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B29">
         <v>45</v>
@@ -1541,30 +1549,30 @@
       <c r="D29">
         <v>40</v>
       </c>
-      <c r="F29">
-        <v>40</v>
+      <c r="F29" t="s">
+        <v>58</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
+        <v>38</v>
+      </c>
+      <c r="B30" t="s">
         <v>39</v>
       </c>
-      <c r="B30" t="s">
+      <c r="C30" t="s">
         <v>40</v>
       </c>
-      <c r="C30" t="s">
+      <c r="D30" t="s">
         <v>41</v>
       </c>
-      <c r="D30" t="s">
-        <v>42</v>
-      </c>
       <c r="F30" t="s">
-        <v>41</v>
+        <v>59</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B31" s="3">
         <v>0.66720000000000002</v>
@@ -1575,47 +1583,47 @@
       <c r="D31" s="3">
         <v>1.0589999999999999</v>
       </c>
-      <c r="F31" s="3">
-        <v>1</v>
+      <c r="F31" s="3" t="s">
+        <v>59</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
+        <v>43</v>
+      </c>
+      <c r="B32" t="s">
         <v>44</v>
       </c>
-      <c r="B32" t="s">
+      <c r="C32" t="s">
         <v>45</v>
       </c>
-      <c r="C32" t="s">
+      <c r="D32" t="s">
         <v>46</v>
       </c>
-      <c r="D32" t="s">
-        <v>47</v>
-      </c>
       <c r="F32" t="s">
-        <v>47</v>
+        <v>58</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
+        <v>47</v>
+      </c>
+      <c r="B33" t="s">
         <v>48</v>
       </c>
-      <c r="B33" t="s">
+      <c r="C33" t="s">
         <v>49</v>
       </c>
-      <c r="C33" t="s">
+      <c r="D33" t="s">
         <v>50</v>
       </c>
-      <c r="D33" t="s">
-        <v>51</v>
-      </c>
       <c r="F33" t="s">
-        <v>51</v>
+        <v>58</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B34">
         <v>125</v>
@@ -1626,30 +1634,30 @@
       <c r="D34">
         <v>50</v>
       </c>
-      <c r="F34">
-        <v>125</v>
+      <c r="F34" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
+        <v>52</v>
+      </c>
+      <c r="B35" t="s">
         <v>53</v>
       </c>
-      <c r="B35" t="s">
+      <c r="C35" t="s">
         <v>54</v>
       </c>
-      <c r="C35" t="s">
+      <c r="D35" t="s">
         <v>55</v>
       </c>
-      <c r="D35" t="s">
-        <v>56</v>
-      </c>
       <c r="F35" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B36">
         <v>17</v>
@@ -1660,8 +1668,8 @@
       <c r="D36">
         <v>24</v>
       </c>
-      <c r="F36">
-        <v>17</v>
+      <c r="F36" t="s">
+        <v>57</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added levels to all the questions
</commit_message>
<xml_diff>
--- a/questions.xlsx
+++ b/questions.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Deepanjaya\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Deepanjaya\Desktop\Computerised-adaptive-assesments\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF4B9A56-785E-49CC-92FD-F94B0A8B89F7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5ED926F6-D7AE-4953-8B34-19942A3FF512}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1046,10 +1046,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F36"/>
+  <dimension ref="A1:G36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="A19" sqref="A19"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="A18" sqref="A18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1057,7 +1057,7 @@
     <col min="1" max="1" width="166.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1073,8 +1073,11 @@
       <c r="F1" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -1090,8 +1093,11 @@
       <c r="F2" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -1107,8 +1113,11 @@
       <c r="F3" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>6</v>
       </c>
@@ -1124,8 +1133,11 @@
       <c r="F4" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>7</v>
       </c>
@@ -1141,8 +1153,11 @@
       <c r="F5" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G5">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>11</v>
       </c>
@@ -1158,8 +1173,11 @@
       <c r="F6" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>12</v>
       </c>
@@ -1175,8 +1193,11 @@
       <c r="F7" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G7">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>13</v>
       </c>
@@ -1192,8 +1213,11 @@
       <c r="F8" s="1" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G8">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>14</v>
       </c>
@@ -1209,8 +1233,11 @@
       <c r="F9" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>15</v>
       </c>
@@ -1226,8 +1253,11 @@
       <c r="F10" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G10">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>16</v>
       </c>
@@ -1243,8 +1273,11 @@
       <c r="F11" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G11">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>17</v>
       </c>
@@ -1260,8 +1293,11 @@
       <c r="F12" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>18</v>
       </c>
@@ -1277,8 +1313,11 @@
       <c r="F13" s="1" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G13">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>19</v>
       </c>
@@ -1294,8 +1333,11 @@
       <c r="F14" s="2" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G14">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>20</v>
       </c>
@@ -1311,8 +1353,11 @@
       <c r="F15" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G15">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>21</v>
       </c>
@@ -1328,8 +1373,11 @@
       <c r="F16" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G16">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>22</v>
       </c>
@@ -1345,8 +1393,11 @@
       <c r="F17" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G17">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>23</v>
       </c>
@@ -1362,8 +1413,11 @@
       <c r="F18" s="3" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="19" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="G18">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A19" s="4" t="s">
         <v>59</v>
       </c>
@@ -1379,8 +1433,11 @@
       <c r="F19" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G19">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>24</v>
       </c>
@@ -1396,8 +1453,11 @@
       <c r="F20" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G20">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>28</v>
       </c>
@@ -1413,8 +1473,11 @@
       <c r="F21" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G21">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>29</v>
       </c>
@@ -1430,8 +1493,11 @@
       <c r="F22" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G22">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>30</v>
       </c>
@@ -1447,8 +1513,11 @@
       <c r="F23" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G23">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>31</v>
       </c>
@@ -1464,8 +1533,11 @@
       <c r="F24" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G24">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>32</v>
       </c>
@@ -1481,8 +1553,11 @@
       <c r="F25" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>33</v>
       </c>
@@ -1498,8 +1573,11 @@
       <c r="F26" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G26">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>34</v>
       </c>
@@ -1515,8 +1593,11 @@
       <c r="F27" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G27">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>35</v>
       </c>
@@ -1532,8 +1613,11 @@
       <c r="F28" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G28">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>36</v>
       </c>
@@ -1549,8 +1633,11 @@
       <c r="F29" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G29">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>37</v>
       </c>
@@ -1566,8 +1653,11 @@
       <c r="F30" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G30">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>41</v>
       </c>
@@ -1583,8 +1673,11 @@
       <c r="F31" s="3" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G31">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>42</v>
       </c>
@@ -1600,8 +1693,11 @@
       <c r="F32" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G32">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>46</v>
       </c>
@@ -1617,8 +1713,11 @@
       <c r="F33" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G33">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>50</v>
       </c>
@@ -1634,8 +1733,11 @@
       <c r="F34" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G34">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>51</v>
       </c>
@@ -1651,8 +1753,11 @@
       <c r="F35" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G35">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>55</v>
       </c>
@@ -1667,6 +1772,9 @@
       </c>
       <c r="F36" t="s">
         <v>58</v>
+      </c>
+      <c r="G36">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
random + restricted entry
</commit_message>
<xml_diff>
--- a/questions.xlsx
+++ b/questions.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\work\BE PROJECT\Computerised-adaptive-assesments\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4261A328-E2D7-47A0-AEBC-F496069E3676}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B99CACA-D2CD-4AC5-ACA6-8289D1DEFFA3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1051,13 +1051,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F36"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:A1048576"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="A22" sqref="A22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="84.140625" customWidth="1"/>
+    <col min="1" max="1" width="118.28515625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Fetch question according to their difficulty level
</commit_message>
<xml_diff>
--- a/questions.xlsx
+++ b/questions.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Deepanjaya\Desktop\Computerised-adaptive-assesments\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5ED926F6-D7AE-4953-8B34-19942A3FF512}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E3A12C7-699A-4A1F-B56B-42F699E1F981}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1049,7 +1049,7 @@
   <dimension ref="A1:G36"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="A18" sqref="A18"/>
+      <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1074,7 +1074,7 @@
         <v>56</v>
       </c>
       <c r="G1">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
@@ -1114,7 +1114,7 @@
         <v>58</v>
       </c>
       <c r="G3">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
@@ -1154,7 +1154,7 @@
         <v>57</v>
       </c>
       <c r="G5">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">

</xml_diff>